<commit_message>
Ultimo commit para presentacion
</commit_message>
<xml_diff>
--- a/src/test/resources/dataDriven/DataVuelos.xlsx
+++ b/src/test/resources/dataDriven/DataVuelos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>ciudadOrigen</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Bogota</t>
+  </si>
+  <si>
+    <t>Medellin</t>
+  </si>
+  <si>
+    <t>Cucuta</t>
   </si>
 </sst>
 </file>
@@ -357,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,6 +412,40 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>